<commit_message>
Refactor malla reading functions to improve header detection and column indexing
- Enhanced `leer_malla_excel_with_sheet` to dynamically detect column indices for "Nombre" and "ID" based on header content.
- Updated logic to skip header rows more robustly and handle empty or malformed rows.
- Introduced atomic static variables for configurable column indices.
- Improved debug logging for better traceability of header detection and row processing.
- Adjusted `leer_malla_con_porcentajes` to utilize new header detection logic and streamline data extraction.
- Added fallback mechanisms for reading names and IDs when they are empty.
- Refactored `leer_malla_con_porcentajes_optimizado` to implement similar header detection and indexing improvements.
- Removed unnecessary legacy code and ensured consistent handling of elective and non-elective courses.
- Added new data files for Malla2010 and Malla2020 with initial content.
</commit_message>
<xml_diff>
--- a/quickshift/src/datafiles/Malla2020.xlsx
+++ b/quickshift/src/datafiles/Malla2020.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="14340" windowHeight="12420"/>
+    <workbookView windowWidth="28740" windowHeight="11010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -202,8 +202,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="23">
@@ -234,9 +234,70 @@
       <charset val="1"/>
     </font>
     <font>
-      <u/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -250,7 +311,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -265,10 +333,10 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -280,39 +348,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -325,7 +363,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -333,50 +370,13 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -387,109 +387,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -501,73 +567,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -605,26 +605,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -644,6 +644,32 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -659,32 +685,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -698,148 +698,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1194,7 +1194,7 @@
   <dimension ref="A1:F57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:F57"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="5"/>

</xml_diff>

<commit_message>
fix: Actualizar archivo Malla2020.xlsx para reflejar cambios en los requisitos
</commit_message>
<xml_diff>
--- a/quickshift/src/datafiles/Malla2020.xlsx
+++ b/quickshift/src/datafiles/Malla2020.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28740" windowHeight="11010"/>
+    <workbookView windowWidth="14400" windowHeight="12600"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -97,7 +97,7 @@
     <t>Desarrollo Web y Móvil</t>
   </si>
   <si>
-    <t>Inglés I</t>
+    <t>Inglés General I</t>
   </si>
   <si>
     <t>Optimización</t>
@@ -112,7 +112,7 @@
     <t>Bases de Datos Avanzadas</t>
   </si>
   <si>
-    <t>Inglés II</t>
+    <t>Inglés General II</t>
   </si>
   <si>
     <t>Contabilidad y Costos</t>
@@ -127,7 +127,7 @@
     <t>Sistemas Operativos</t>
   </si>
   <si>
-    <t>Inglés III</t>
+    <t>Inglés General III</t>
   </si>
   <si>
     <t>Gestión Organizacional</t>
@@ -201,10 +201,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -234,6 +234,14 @@
       <charset val="1"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -243,10 +251,32 @@
     </font>
     <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -265,31 +295,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -304,7 +319,31 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -324,9 +363,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -334,49 +372,11 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -387,19 +387,115 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -411,163 +507,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -608,22 +608,31 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
+      <right style="double">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
+      <top style="double">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
+      <bottom style="double">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -640,32 +649,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -687,9 +670,26 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -698,148 +698,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1193,8 +1193,8 @@
   <sheetPr/>
   <dimension ref="A1:F57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="5"/>
@@ -1639,7 +1639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" ht="15.75" spans="1:6">
+    <row r="22" ht="29.25" spans="1:6">
       <c r="A22" s="2" t="s">
         <v>27</v>
       </c>
@@ -1765,7 +1765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" ht="15.75" spans="1:6">
+    <row r="28" ht="29.25" spans="1:6">
       <c r="A28" s="2" t="s">
         <v>32</v>
       </c>
@@ -1891,7 +1891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" ht="15.75" spans="1:6">
+    <row r="34" ht="43.5" spans="1:6">
       <c r="A34" s="2" t="s">
         <v>37</v>
       </c>

</xml_diff>